<commit_message>
Simplify report generation window
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel_template_full.xlsx
+++ b/src/main/resources/templates/excel_template_full.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="13350"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Фамилия</t>
   </si>
@@ -32,15 +32,6 @@
   </si>
   <si>
     <t>Колличество ужинов</t>
-  </si>
-  <si>
-    <t>Стоимость обедов</t>
-  </si>
-  <si>
-    <t>Стоимость ужинов</t>
-  </si>
-  <si>
-    <t>Общая стоимость</t>
   </si>
   <si>
     <t>№</t>
@@ -52,8 +43,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -113,9 +104,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -128,9 +122,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -168,7 +162,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -202,7 +196,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,10 +230,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -413,17 +405,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
@@ -437,9 +429,9 @@
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18.75">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -447,13 +439,13 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="42" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -472,20 +464,11 @@
       </c>
       <c r="G2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>